<commit_message>
Finished InsertImageIn Excel Task.
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/InsertImage.xlsx
+++ b/src/main/java/resources/excelsheet/InsertImage.xlsx
@@ -7,12 +7,48 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>TC_1</t>
+  </si>
+  <si>
+    <t>TC_2</t>
+  </si>
+  <si>
+    <t>TC_3</t>
+  </si>
+  <si>
+    <t>TC_4</t>
+  </si>
+  <si>
+    <t>TC_5</t>
+  </si>
+  <si>
+    <t>TC_6</t>
+  </si>
+  <si>
+    <t>TC_7</t>
+  </si>
+  <si>
+    <t>TC_8</t>
+  </si>
+  <si>
+    <t>TC_9</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>TestCases</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,38 +385,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>